<commit_message>
Agregue el archivo de estadisticas
</commit_message>
<xml_diff>
--- a/ReportesDeConsultaApi/datos_de_monedas.xlsx
+++ b/ReportesDeConsultaApi/datos_de_monedas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,12 +494,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1.24</t>
+          <t>-1.64</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.82</t>
+          <t>1.58</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>21888438965.2427</v>
+        <v>20016432062.50752</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -542,21 +542,21 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.91</t>
+          <t>-2.46</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-4.92</t>
+          <t>-3.45</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.049107</t>
+          <t>0.048635</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>7671839281.724711</v>
+        <v>7983191628.563033</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -586,12 +586,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-0.16</t>
+          <t>-0.08</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-0.21</t>
+          <t>0.11</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>35546961159.60201</v>
+        <v>33444475110.36345</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -630,21 +630,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.63</t>
+          <t>-0.96</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-2.38</t>
+          <t>-0.88</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.009249</t>
+          <t>0.009291</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>405898180.4503363</v>
+        <v>374558566.2793692</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.32</t>
+          <t>3.22</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>3.39</t>
+          <t>12.19</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.002291</t>
+          <t>0.002405</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>1662462500.162592</v>
+        <v>1360327736.400119</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -727,7 +727,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>-0.06</t>
+          <t>-0.01</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>2567111696.102907</v>
+        <v>2246820917.771317</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -766,21 +766,21 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>-2.47</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>-4.96</t>
+          <t>-3.56</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.049028</t>
+          <t>0.048537</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>62843401.58366791</v>
+        <v>46700884.55244054</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -796,17 +796,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>58</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dogecoin</t>
+          <t>ripple</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -814,43 +814,47 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3.76</t>
+          <t>6.46</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>10.01</t>
+          <t>11.63</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.000003</t>
+          <t>0.000009</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>2554294158.183266</v>
+        <v>543441707.2980735</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>144031626384.00</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr"/>
+          <t>42909539227.00</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>100000000000</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ripple</t>
+          <t>dogecoin</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -858,32 +862,28 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.88</t>
+          <t>-4.20</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2.59</t>
+          <t>8.36</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.000008</t>
+          <t>0.000002</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>655569133.8958174</v>
+        <v>1480232398.43884</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>42909539227.00</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>100000000000</t>
-        </is>
-      </c>
+          <t>144031626384.00</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -906,12 +906,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>4.41</t>
+          <t>-1.20</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>7.66</t>
+          <t>9.96</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>119536125.9955335</v>
+        <v>122839095.6267197</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -954,12 +954,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.51</t>
+          <t>0.10</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>-2.38</t>
+          <t>2.06</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>227877285.872933</v>
+        <v>216677443.6232141</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1002,21 +1002,21 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.64</t>
+          <t>-2.95</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0.95</t>
+          <t>1.70</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3.90E-10</t>
+          <t>3.82E-10</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>58443420.34874169</v>
+        <v>46207305.30115544</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1046,21 +1046,21 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>-0.27</t>
+          <t>-0.50</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>8.12</t>
+          <t>11.39</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0.000583</t>
+          <t>0.000590</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>332364932.5959993</v>
+        <v>328898372.9548351</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1094,12 +1094,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>-0.09</t>
+          <t>-1.93</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0.38</t>
+          <t>-0.90</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1108,7 +1108,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>288737255.7402035</v>
+        <v>263014982.1162345</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1138,21 +1138,21 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>-1.56</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0.48</t>
+          <t>1.28</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0.998779</t>
+          <t>0.997922</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>67507679.84846112</v>
+        <v>30536390.34339679</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1164,17 +1164,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>45219</t>
+          <t>2321</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>DOT</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>polkadot</t>
+          <t>bitcoin-cash</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1182,47 +1182,47 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2.29</t>
+          <t>2.60</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>6.19</t>
+          <t>4.13</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.000113</t>
+          <t>0.007614</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>148404014.6360258</v>
+        <v>302596326.9808153</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>1307052068.00</t>
+          <t>19696959.00</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>1388001203.0802</t>
+          <t>21000000</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2321</t>
+          <t>45219</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BCH</t>
+          <t>DOT</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>bitcoin-cash</t>
+          <t>polkadot</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1230,30 +1230,30 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.81</t>
+          <t>-0.89</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>-2.30</t>
+          <t>7.53</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0.007317</t>
+          <t>0.000113</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>370722872.4091192</v>
+        <v>147153744.2166693</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>19696959.00</t>
+          <t>1307052068.00</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>21000000</t>
+          <t>1388001203.0802</t>
         </is>
       </c>
     </row>
@@ -1278,21 +1278,21 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.18</t>
+          <t>1.05</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>1.62</t>
+          <t>4.60</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0.000224</t>
+          <t>0.000232</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>217563913.9572769</v>
+        <v>172420433.170528</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1326,12 +1326,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>7.60</t>
+          <t>-2.99</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>-0.61</t>
+          <t>4.68</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1340,7 +1340,7 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>268435594.3003821</v>
+        <v>371242586.4062572</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1374,21 +1374,21 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.34</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>-4.06</t>
+          <t>-2.50</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0.001267</t>
+          <t>0.001291</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>375494216.3643599</v>
+        <v>379296161.9463164</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1400,6 +1400,1124 @@
           <t>84000000</t>
         </is>
       </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>33833</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>unus-sed-leo</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>21</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-0.23</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>1.43</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>0.000092</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>4845195.416932933</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>927132386.00</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>47305</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>UNI</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>uniswap</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>22</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-1.62</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>0.000119</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>76647434.95116875</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>598736139.00</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>1000000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ETC</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ethereum-classic</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>23</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>-0.86</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>0.32</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>0.000434</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>305772815.4121829</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>145903895.00</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>210700000</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>33830</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ATOM</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>cosmos</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>24</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1.38</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>15.89</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>0.000148</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>99489558.74172102</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>389254388.00</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>44863</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>RNDR</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>render-token</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>25</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>-0.92</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>22.17</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>0.000153</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>246852404.6089281</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>374355803.00</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>536870912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>93841</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>PEPE</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>pepe</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>26</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>23.12</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1.35E-10</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>10435685.48656852</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>420689899999990.00</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>420690000000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>121595</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>MNT</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>mantle</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>27</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>-1.55</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-0.79</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>0.000017</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>43832408.0898506</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>3231662126.00</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>6219316795</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>121613</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>dogwifhat</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>28</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2.56</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>27.31</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0.000053</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>124346136.1753015</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>998920172.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>111341</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>APT</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>aptos</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>29</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>-1.76</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>1.05</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0.000144</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>85269915.8665657</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>368468672.00</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>1084577363.9802</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>XLM</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>stellar</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>30</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>1.91</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>1.02</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>0.000002</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>39231767.64845359</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>28919327940.00</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>104303927518</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>48569</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>STX</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>stacks</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>31</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>-5.12</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>-8.94</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>0.000035</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>88118251.47747172</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>1444838084.00</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>1818000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>32607</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>FIL</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>filecoin</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>32</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>-1.95</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>4.73</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>0.000097</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>134456002.2005726</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>519800264.00</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>100423</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>FDUSD</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>first-digital-usd</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>33</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>-0.01</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>0.000016</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>3721160459.763143</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>3098764893.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>121593</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>IMX</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>immutable-x</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>34</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>-3.26</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>6.29</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>0.000035</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>35560177.32694522</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>1389224659.00</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>2000000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>33531</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>OKB</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>okb</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>35</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-2.37</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>-1.92</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>0.000799</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>5986769.208649665</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>60000000.00</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>96901</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>WBETH</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>wrapped-beacon-eth</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>36</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>-2.38</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>-3.31</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>0.050493</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>2523238.282378155</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>889399.00</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>889399.86447924</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>121619</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>TAO</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>bittensor</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>37</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>-6.07</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>7.09</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>0.006995</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>15152072.00573391</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>6374044.00</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>21000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>48561</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>GRT</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>the-graph</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>38</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>-5.04</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>12.55</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>0.000004</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>118718225.013203</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>9417713956.00</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2741</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>VET</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>vechain</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>39</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>-3.29</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>-6.99</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>5.75E-7</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>38338821.43712051</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>72714516834.00</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>86712634466</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>42441</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>arweave</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>40</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>-3.41</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>10.51</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>0.000628</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>221857179.4204142</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>65454185.00</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>66000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>12377</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>MKR</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>maker</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>41</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>-4.17</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>-6.32</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>0.044436</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>71650779.25092077</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>923569.00</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>1005577</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>70497</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>OP</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>optimism</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>42</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>-3.54</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>8.58</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>0.000044</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>199567232.0431302</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>911294948.00</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>4294967296</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>70485</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>KAS</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>kaspa</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>43</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0.93</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>-4.74</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>0.000002</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>25692179.64992524</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>22926816511.00</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>28704026601</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>XMR</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>monero</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>44</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0.94</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>4.60</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>0.002061</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>1162232808.347799</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>18406889.00</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
separado de funcion dato
</commit_message>
<xml_diff>
--- a/ReportesDeConsultaApi/datos_de_monedas.xlsx
+++ b/ReportesDeConsultaApi/datos_de_monedas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,12 +494,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-1.64</t>
+          <t>0.35</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1.58</t>
+          <t>0.21</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>20016432062.50752</v>
+        <v>27467658598.48648</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -542,21 +542,21 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-2.46</t>
+          <t>-0.42</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-3.45</t>
+          <t>-3.36</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.048635</t>
+          <t>0.048270</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>7983191628.563033</v>
+        <v>10771076454.20971</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -586,12 +586,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-0.08</t>
+          <t>-0.05</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.11</t>
+          <t>-0.30</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>33444475110.36345</v>
+        <v>44835413287.13708</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -630,21 +630,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-0.96</t>
+          <t>0.84</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-0.88</t>
+          <t>-1.25</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.009291</t>
+          <t>0.009344</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>374558566.2793692</v>
+        <v>501162059.1712992</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3.22</t>
+          <t>1.29</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>12.19</t>
+          <t>13.73</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.002405</t>
+          <t>0.002423</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>1360327736.400119</v>
+        <v>2499304258.724568</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -722,7 +722,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.01</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>2246820917.771317</v>
+        <v>3437834993.044488</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -766,21 +766,21 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-2.47</t>
+          <t>-0.42</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>-3.56</t>
+          <t>-3.40</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.048537</t>
+          <t>0.048193</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>46700884.55244054</v>
+        <v>81584646.67647275</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -814,12 +814,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>6.46</t>
+          <t>-1.86</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>11.63</t>
+          <t>5.31</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -828,7 +828,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>543441707.2980735</v>
+        <v>1443695100.808488</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -862,12 +862,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-4.20</t>
+          <t>-0.34</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>8.36</t>
+          <t>8.73</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>1480232398.43884</v>
+        <v>1428667307.267194</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -906,12 +906,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-1.20</t>
+          <t>-0.78</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>9.96</t>
+          <t>9.50</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>122839095.6267197</v>
+        <v>179048558.5134867</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -954,12 +954,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.10</t>
+          <t>-2.01</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2.06</t>
+          <t>-0.59</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>216677443.6232141</v>
+        <v>293771116.1444727</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1002,21 +1002,21 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>-2.95</t>
+          <t>-1.54</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>1.70</t>
+          <t>-0.81</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3.82E-10</t>
+          <t>3.74E-10</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>46207305.30115544</v>
+        <v>65258366.33592062</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1046,21 +1046,21 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>-0.50</t>
+          <t>-1.10</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>11.39</t>
+          <t>6.22</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0.000590</t>
+          <t>0.000580</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>328898372.9548351</v>
+        <v>408026138.0630771</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1094,12 +1094,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>-1.93</t>
+          <t>1.55</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>-0.90</t>
+          <t>0.75</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1108,7 +1108,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>263014982.1162345</v>
+        <v>356722804.212838</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1138,21 +1138,21 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>-1.56</t>
+          <t>0.33</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>1.28</t>
+          <t>0.03</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0.997922</t>
+          <t>0.998031</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>30536390.34339679</v>
+        <v>72781170.93854488</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1182,21 +1182,21 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2.60</t>
+          <t>1.37</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>4.13</t>
+          <t>5.22</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.007614</t>
+          <t>0.007661</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>302596326.9808153</v>
+        <v>373318882.4025794</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1230,12 +1230,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>-0.89</t>
+          <t>-0.25</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>7.53</t>
+          <t>9.40</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1244,7 +1244,7 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>147153744.2166693</v>
+        <v>216505614.6039383</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1278,21 +1278,21 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.05</t>
+          <t>-1.79</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>4.60</t>
+          <t>3.11</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0.000232</t>
+          <t>0.000226</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>172420433.170528</v>
+        <v>279710790.4686785</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1326,21 +1326,21 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>-2.99</t>
+          <t>2.06</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>4.68</t>
+          <t>8.79</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0.000114</t>
+          <t>0.000116</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>371242586.4062572</v>
+        <v>438773796.3666959</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1374,21 +1374,21 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.34</t>
+          <t>0.78</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>-2.50</t>
+          <t>-1.04</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0.001291</t>
+          <t>0.001296</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>379296161.9463164</v>
+        <v>501731536.8528561</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1422,21 +1422,21 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>-0.23</t>
+          <t>0.77</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>1.43</t>
+          <t>-0.52</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0.000092</t>
+          <t>0.000091</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>4845195.416932933</v>
+        <v>3494352.94133756</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1466,12 +1466,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.15</t>
+          <t>0.44</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>-1.62</t>
+          <t>-1.10</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1480,7 +1480,7 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>76647434.95116875</v>
+        <v>96116606.67136998</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1514,21 +1514,21 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>-0.86</t>
+          <t>0.62</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0.32</t>
+          <t>1.18</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0.000434</t>
+          <t>0.000435</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>305772815.4121829</v>
+        <v>400749386.7501777</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1544,17 +1544,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>33830</t>
+          <t>44863</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ATOM</t>
+          <t>RNDR</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>cosmos</t>
+          <t>render-token</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1562,43 +1562,47 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.38</t>
+          <t>10.58</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>15.89</t>
+          <t>38.86</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>0.000148</t>
+          <t>0.000169</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>99489558.74172102</v>
+        <v>309027174.4896991</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>389254388.00</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr"/>
+          <t>374355803.00</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>536870912</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>44863</t>
+          <t>33830</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>RNDR</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>render-token</t>
+          <t>cosmos</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1606,32 +1610,28 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>-0.92</t>
+          <t>-0.90</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>22.17</t>
+          <t>14.27</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>0.000153</t>
+          <t>0.000147</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>246852404.6089281</v>
+        <v>154170773.6204464</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>374355803.00</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>536870912</t>
-        </is>
-      </c>
+          <t>389254388.00</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1654,21 +1654,21 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.35</t>
+          <t>-3.17</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>23.12</t>
+          <t>12.32</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>1.35E-10</t>
+          <t>1.30E-10</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>10435685.48656852</v>
+        <v>9423581.166320723</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1702,12 +1702,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>-1.55</t>
+          <t>1.12</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>-0.79</t>
+          <t>3.38</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1716,7 +1716,7 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>43832408.0898506</v>
+        <v>46941195.31005198</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -1750,12 +1750,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2.56</t>
+          <t>-0.18</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>27.31</t>
+          <t>27.64</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1764,7 +1764,7 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>124346136.1753015</v>
+        <v>186818305.9748314</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1793,21 +1793,21 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>-1.76</t>
+          <t>-0.50</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>1.05</t>
+          <t>1.04</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>0.000144</t>
+          <t>0.000142</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>85269915.8665657</v>
+        <v>118341616.0648232</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -1823,17 +1823,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>48569</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>XLM</t>
+          <t>STX</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>stellar</t>
+          <t>stacks</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1841,47 +1841,47 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.91</t>
+          <t>1.60</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>1.02</t>
+          <t>-6.92</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>0.000002</t>
+          <t>0.000035</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>39231767.64845359</v>
+        <v>102958474.3427878</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>28919327940.00</t>
+          <t>1444838084.00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>104303927518</t>
+          <t>1818000000</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>48569</t>
+          <t>89</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>STX</t>
+          <t>XLM</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>stacks</t>
+          <t>stellar</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1889,30 +1889,30 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>-5.12</t>
+          <t>-1.98</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>-8.94</t>
+          <t>-1.62</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>0.000035</t>
+          <t>0.000002</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>88118251.47747172</v>
+        <v>74872961.83501349</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>1444838084.00</t>
+          <t>28919327940.00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>1818000000</t>
+          <t>104303927518</t>
         </is>
       </c>
     </row>
@@ -1937,21 +1937,21 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>-1.95</t>
+          <t>-2.20</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>4.73</t>
+          <t>1.87</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>0.000097</t>
+          <t>0.000094</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>134456002.2005726</v>
+        <v>187135716.1690417</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -1981,12 +1981,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>-0.01</t>
+          <t>0.04</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>0.07</t>
+          <t>0.05</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1995,529 +1995,13 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>3721160459.763143</v>
+        <v>5976846372.116722</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
           <t>3098764893.00</t>
         </is>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>121593</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>IMX</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>immutable-x</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>34</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>-3.26</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>6.29</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>0.000035</t>
-        </is>
-      </c>
-      <c r="H35" t="n">
-        <v>35560177.32694522</v>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>1389224659.00</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>2000000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>33531</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>OKB</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>okb</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>35</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>-2.37</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>-1.92</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>0.000799</t>
-        </is>
-      </c>
-      <c r="H36" t="n">
-        <v>5986769.208649665</v>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>60000000.00</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr"/>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>96901</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>WBETH</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>wrapped-beacon-eth</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>36</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>-2.38</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>-3.31</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>0.050493</t>
-        </is>
-      </c>
-      <c r="H37" t="n">
-        <v>2523238.282378155</v>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>889399.00</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>889399.86447924</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>121619</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>bittensor</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>37</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>-6.07</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>7.09</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>0.006995</t>
-        </is>
-      </c>
-      <c r="H38" t="n">
-        <v>15152072.00573391</v>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>6374044.00</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>21000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>48561</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>GRT</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>the-graph</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>38</v>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>-5.04</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>12.55</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>0.000004</t>
-        </is>
-      </c>
-      <c r="H39" t="n">
-        <v>118718225.013203</v>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>9417713956.00</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>2741</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>VET</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>vechain</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>39</v>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>-3.29</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>-6.99</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>5.75E-7</t>
-        </is>
-      </c>
-      <c r="H40" t="n">
-        <v>38338821.43712051</v>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>72714516834.00</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>86712634466</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>42441</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>AR</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>arweave</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>40</v>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>-3.41</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>10.51</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>0.000628</t>
-        </is>
-      </c>
-      <c r="H41" t="n">
-        <v>221857179.4204142</v>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>65454185.00</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>66000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>12377</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>MKR</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>maker</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>41</v>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>-4.17</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>-6.32</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>0.044436</t>
-        </is>
-      </c>
-      <c r="H42" t="n">
-        <v>71650779.25092077</v>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>923569.00</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>1005577</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>70497</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>OP</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>optimism</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>42</v>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>-3.54</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>8.58</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>0.000044</t>
-        </is>
-      </c>
-      <c r="H43" t="n">
-        <v>199567232.0431302</v>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>911294948.00</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>4294967296</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>70485</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>KAS</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>kaspa</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>43</v>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>0.93</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>-4.74</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>0.000002</t>
-        </is>
-      </c>
-      <c r="H44" t="n">
-        <v>25692179.64992524</v>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>22926816511.00</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>28704026601</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>XMR</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>monero</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>44</v>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>0.94</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>4.60</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>0.002061</t>
-        </is>
-      </c>
-      <c r="H45" t="n">
-        <v>1162232808.347799</v>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>18406889.00</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
try-except con funcion coins
</commit_message>
<xml_diff>
--- a/ReportesDeConsultaApi/datos_de_monedas.xlsx
+++ b/ReportesDeConsultaApi/datos_de_monedas.xlsx
@@ -494,12 +494,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-2.46</t>
+          <t>-1.61</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2.76</t>
+          <t>4.28</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>27706121424.34338</v>
+        <v>27432954554.97071</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -542,21 +542,21 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-2.14</t>
+          <t>-1.53</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-0.09</t>
+          <t>1.21</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.048631</t>
+          <t>0.048538</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>10872866959.89374</v>
+        <v>10698834803.34144</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -586,12 +586,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>-0.03</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-0.05</t>
+          <t>-0.03</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>42696684463.78299</v>
+        <v>42317824494.95636</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -630,21 +630,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-1.46</t>
+          <t>-1.09</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1.59</t>
+          <t>2.74</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.009433</t>
+          <t>0.009398</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>516075947.270789</v>
+        <v>518175263.1813599</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-5.59</t>
+          <t>-3.87</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>15.18</t>
+          <t>18.50</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.002364</t>
+          <t>0.002371</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>2625646071.502049</v>
+        <v>2579851111.428535</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>3533122222.121038</v>
+        <v>3499145249.343101</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -766,21 +766,21 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-2.03</t>
+          <t>-1.55</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>1.16</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.048626</t>
+          <t>0.048478</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>86083140.05802134</v>
+        <v>86071853.94508265</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -814,12 +814,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-2.66</t>
+          <t>-2.47</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>4.45</t>
+          <t>5.36</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -828,7 +828,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>1569888933.62219</v>
+        <v>1573477918.634741</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -862,12 +862,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-5.41</t>
+          <t>-4.15</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>13.08</t>
+          <t>15.70</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>1140779107.791037</v>
+        <v>1115770111.721719</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -906,21 +906,21 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-2.65</t>
+          <t>-1.37</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>12.25</t>
+          <t>14.28</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0.000093</t>
+          <t>0.000094</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>112181376.3982848</v>
+        <v>108421926.3558878</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -954,12 +954,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-2.47</t>
+          <t>-1.37</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>1.90</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>284066981.3538923</v>
+        <v>282407397.525009</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
cambio forma de ruta -ok
</commit_message>
<xml_diff>
--- a/ReportesDeConsultaApi/datos_de_monedas.xlsx
+++ b/ReportesDeConsultaApi/datos_de_monedas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,12 +494,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-1.32</t>
+          <t>-0.84</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>4.65</t>
+          <t>2.33</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>27351831684.30545</v>
+        <v>25568135826.20729</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -542,21 +542,21 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-1.32</t>
+          <t>-1.68</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1.38</t>
+          <t>-2.65</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.048334</t>
+          <t>0.048056</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>10640178744.71991</v>
+        <v>9686944591.17938</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -586,12 +586,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.26</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-0.03</t>
+          <t>0.07</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>42158352089.12697</v>
+        <v>40696530706.8419</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -630,21 +630,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-0.72</t>
+          <t>-2.06</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2.82</t>
+          <t>3.63</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.009361</t>
+          <t>0.009587</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>516654625.4563156</v>
+        <v>732817438.2325318</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-3.50</t>
+          <t>1.47</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>18.53</t>
+          <t>4.84</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.002368</t>
+          <t>0.002405</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>2543974618.38427</v>
+        <v>2085982378.587099</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -722,12 +722,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>-0.03</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>-0.09</t>
+          <t>0.03</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>3494405717.586186</v>
+        <v>3064675682.500233</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -766,21 +766,21 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-1.34</t>
+          <t>-1.56</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1.52</t>
+          <t>-2.37</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.048272</t>
+          <t>0.048034</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>85519479.80683161</v>
+        <v>46546039.83994892</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -796,17 +796,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>54683</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>TON Coin</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -814,47 +814,47 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-1.86</t>
+          <t>11.55</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>5.37</t>
+          <t>27.01</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.000008</t>
+          <t>0.000110</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>1578910784.920042</v>
+        <v>191294892.0892293</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>42909539227.00</t>
+          <t>3468312277.00</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>100000000000</t>
+          <t>5047558528</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>58</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DOGE</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dogecoin</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -862,43 +862,47 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-3.54</t>
+          <t>-2.44</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>15.59</t>
+          <t>-3.98</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.000002</t>
+          <t>0.000008</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>1107319867.357455</v>
+        <v>947838748.1660337</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>144031626384.00</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr"/>
+          <t>42909539227.00</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>100000000000</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>54683</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>DOGE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>TON Coin</t>
+          <t>Dogecoin</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -906,32 +910,28 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>-2.22</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>16.92</t>
+          <t>7.76</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0.000094</t>
+          <t>0.000002</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>107012041.0182199</v>
+        <v>969776173.8468813</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3468312277.00</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>5047558528</t>
-        </is>
-      </c>
+          <t>144031626384.00</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -954,12 +954,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.28</t>
+          <t>-0.79</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2.92</t>
+          <t>-2.63</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>280953109.5084246</v>
+        <v>403263516.0196248</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -978,518 +978,6 @@
       <c r="J12" t="inlineStr">
         <is>
           <t>45000000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>45088</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>SHIB</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Shiba Inu</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>12</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>-2.59</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>5.51</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>3.69E-10</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>55970131.3870844</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>589289410812691.00</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>44883</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>AVAX</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Avalanche</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>13</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>-4.72</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>7.63</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>0.000558</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>322363867.8346865</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>377285092.00</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>720000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2713</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>TRX</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>TRON</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>14</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2.03</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2.04</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>0.000002</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>369174214.0909887</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>87923847381.00</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>33422</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>WBTC</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Wrapped Bitcoin</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>15</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>-1.17</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>4.65</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>0.999055</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>64431223.27477978</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>155986.00</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>45219</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>DOT</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Polkadot</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>16</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>-0.49</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>10.88</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>0.000114</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>163021423.5851867</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>1307052068.00</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>1388001203.0802</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2321</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>BCH</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Bitcoin Cash</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>17</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>-3.79</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>9.77</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>0.007452</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>409097021.9790089</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>19696959.00</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>21000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2751</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>LINK</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>ChainLink</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>18</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>-3.63</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>7.44</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>0.000224</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>263555256.9331217</v>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>587099970.00</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>1000000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>48563</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>NEAR</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>NEAR Protocol</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>19</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>-3.97</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>16.34</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>0.000115</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>542327508.8163048</v>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>1043761976.00</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>1043761976</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>LTC</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Litecoin</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>20</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>3.60</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>0.001308</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>451549391.6600372</v>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>74461469.00</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>84000000</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>33833</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>UNUS SED LEO</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>21</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>1.30</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>1.02</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>0.000094</t>
-        </is>
-      </c>
-      <c r="H22" t="n">
-        <v>3387099.824175597</v>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>927132386.00</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>47305</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>UNI</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Uniswap</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>22</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>-0.59</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>6.78</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>0.000120</t>
-        </is>
-      </c>
-      <c r="H23" t="n">
-        <v>82075598.55814226</v>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>598736139.00</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>1000000000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
incluir la consulta sin internet
</commit_message>
<xml_diff>
--- a/ReportesDeConsultaApi/datos_de_monedas.xlsx
+++ b/ReportesDeConsultaApi/datos_de_monedas.xlsx
@@ -494,12 +494,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2.43</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-5.08</t>
+          <t>-1.73</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>15273751475.60659</v>
+        <v>16811111921.82245</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -542,21 +542,21 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-1.43</t>
+          <t>2.30</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-8.49</t>
+          <t>-4.67</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.047270</t>
+          <t>0.047138</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>5465494719.420193</v>
+        <v>5910814763.210913</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -586,12 +586,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>-0.01</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>-0.34</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>25365550976.63667</v>
+        <v>26301615210.77409</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -630,21 +630,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-0.54</t>
+          <t>0.09</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-1.12</t>
+          <t>0.01</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.009628</t>
+          <t>0.009406</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>342903945.8178671</v>
+        <v>396894481.6348014</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-5.34</t>
+          <t>4.12</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>-5.50</t>
+          <t>-4.84</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.002273</t>
+          <t>0.002342</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>965914975.0185841</v>
+        <v>1028603983.755987</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -727,7 +727,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>0.04</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>2177645892.003948</v>
+        <v>1947232075.422707</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -766,21 +766,21 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-1.40</t>
+          <t>2.30</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>-8.41</t>
+          <t>-4.79</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.047247</t>
+          <t>0.047105</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>28404951.01139832</v>
+        <v>31166623.05574772</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -814,21 +814,21 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-0.72</t>
+          <t>0.75</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>16.15</t>
+          <t>17.24</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.000113</t>
+          <t>0.000111</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>228478526.0475519</v>
+        <v>257667042.5942079</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -862,12 +862,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-3.18</t>
+          <t>2.69</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>-7.58</t>
+          <t>-4.89</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>402981619.8243122</v>
+        <v>476588212.4435817</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -910,12 +910,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-5.12</t>
+          <t>8.34</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>-15.22</t>
+          <t>-5.82</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -924,7 +924,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>408629332.9242619</v>
+        <v>546804803.228668</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -954,12 +954,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-3.15</t>
+          <t>1.38</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>-7.72</t>
+          <t>-4.82</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>152405279.3259398</v>
+        <v>150783742.4091178</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>

</xml_diff>